<commit_message>
Just a couple of touches here and there
</commit_message>
<xml_diff>
--- a/backlog - dissertation.xlsx
+++ b/backlog - dissertation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>Task</t>
   </si>
@@ -69,6 +69,21 @@
   </si>
   <si>
     <t>example: lazy/strict signal, dependency</t>
+  </si>
+  <si>
+    <t>Scala.Swing</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>explain event mechanism</t>
+  </si>
+  <si>
+    <t>IN PROGRESS</t>
+  </si>
+  <si>
+    <t>add line drawing demo to appendix</t>
   </si>
 </sst>
 </file>
@@ -124,9 +139,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C10" totalsRowShown="0">
-  <autoFilter ref="A1:C10"/>
-  <sortState ref="A2:C10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C13" totalsRowShown="0">
+  <autoFilter ref="A1:C13"/>
+  <sortState ref="A2:C13">
     <sortCondition ref="A2:A10"/>
   </sortState>
   <tableColumns count="3">
@@ -401,16 +416,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.88671875" customWidth="1"/>
     <col min="2" max="2" width="33.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -482,17 +498,44 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Worked a lot on FEST-Logging
</commit_message>
<xml_diff>
--- a/backlog - dissertation.xlsx
+++ b/backlog - dissertation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>Task</t>
   </si>
@@ -80,9 +80,6 @@
     <t>explain event mechanism</t>
   </si>
   <si>
-    <t>IN PROGRESS</t>
-  </si>
-  <si>
     <t>add line drawing demo to appendix</t>
   </si>
   <si>
@@ -90,6 +87,33 @@
   </si>
   <si>
     <t>explain the features</t>
+  </si>
+  <si>
+    <t>change the UMLs to Visio PDFs</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>Generic</t>
+  </si>
+  <si>
+    <t>Drag-and-drop</t>
+  </si>
+  <si>
+    <t>explain how sim. drag and drop works</t>
+  </si>
+  <si>
+    <t>Overview</t>
+  </si>
+  <si>
+    <t>rework the overview</t>
+  </si>
+  <si>
+    <t>Abstract</t>
+  </si>
+  <si>
+    <t>rework the abstract</t>
   </si>
 </sst>
 </file>
@@ -145,11 +169,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C15" totalsRowShown="0">
-  <autoFilter ref="A1:C15"/>
-  <sortState ref="A2:C13">
-    <sortCondition ref="A2:A10"/>
-  </sortState>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C19" totalsRowShown="0">
   <tableColumns count="3">
     <tableColumn id="1" name="Section"/>
     <tableColumn id="2" name="Task"/>
@@ -422,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -448,117 +468,158 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>6</v>
       </c>
-      <c r="B15" t="s">
-        <v>21</v>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work on Scala, introduced type hierarchy and partial functions, and cleaned up the rest
</commit_message>
<xml_diff>
--- a/backlog - dissertation.xlsx
+++ b/backlog - dissertation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
   <si>
     <t>Task</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t xml:space="preserve">explain the solved issues </t>
+  </si>
+  <si>
+    <t>rework the general structure</t>
   </si>
 </sst>
 </file>
@@ -181,10 +184,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D21" totalsRowShown="0">
-  <sortState ref="A2:D21">
-    <sortCondition ref="C2:C21"/>
-    <sortCondition ref="A2:A21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D22" totalsRowShown="0">
+  <sortState ref="A2:D22">
+    <sortCondition ref="C2:C22"/>
+    <sortCondition ref="A2:A22"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" name="Section"/>
@@ -459,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -584,21 +587,24 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C9">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C10">
         <v>10</v>
@@ -606,10 +612,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -617,13 +623,16 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -631,7 +640,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -639,10 +648,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C14">
         <v>10</v>
@@ -650,10 +659,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C15">
         <v>10</v>
@@ -661,67 +670,81 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>23</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>21</v>
-      </c>
-      <c r="C16">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" t="s">
-        <v>4</v>
       </c>
       <c r="C17">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C18">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C19">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>6</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>19</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding the line drawing example to the appendix
</commit_message>
<xml_diff>
--- a/backlog - dissertation.xlsx
+++ b/backlog - dissertation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
   <si>
     <t>Task</t>
   </si>
@@ -645,6 +645,9 @@
       <c r="C13">
         <v>10</v>
       </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">

</xml_diff>

<commit_message>
Removing simulated drag and drop...
</commit_message>
<xml_diff>
--- a/backlog - dissertation.xlsx
+++ b/backlog - dissertation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
   <si>
     <t>Task</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>rework the general structure</t>
+  </si>
+  <si>
+    <t>DEFERRED</t>
   </si>
 </sst>
 </file>
@@ -465,7 +468,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -609,6 +612,9 @@
       <c r="C10">
         <v>10</v>
       </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">

</xml_diff>

<commit_message>
Close to being final
</commit_message>
<xml_diff>
--- a/backlog - dissertation.xlsx
+++ b/backlog - dissertation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="49">
   <si>
     <t>Task</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t>consider using the original paragraph style</t>
+  </si>
+  <si>
+    <t>Scala CPS Plugin</t>
+  </si>
+  <si>
+    <t>Reference programming with shift/reset</t>
   </si>
 </sst>
 </file>
@@ -220,13 +226,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D33" totalsRowShown="0">
-  <autoFilter ref="A1:D33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D34" totalsRowShown="0">
+  <autoFilter ref="A1:D34">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>
-  <sortState ref="A13:D33">
+  <sortState ref="A13:D34">
     <sortCondition ref="C2:C32"/>
     <sortCondition ref="A2:A32"/>
   </sortState>
@@ -503,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -869,7 +875,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -878,6 +884,9 @@
       </c>
       <c r="C27">
         <v>15</v>
+      </c>
+      <c r="D27" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -896,56 +905,76 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="C29">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>12</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C30">
         <v>15</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C31">
         <v>15</v>
       </c>
+      <c r="D31" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>23</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>21</v>
       </c>
-      <c r="C32">
+      <c r="C33">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="D33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>6</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>19</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New title, somewhat refined introduction.
</commit_message>
<xml_diff>
--- a/backlog - dissertation.xlsx
+++ b/backlog - dissertation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="50">
   <si>
     <t>Task</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>Reference programming with shift/reset</t>
+  </si>
+  <si>
+    <t>Explain the connection between Scala.Reat and CPS transformation</t>
   </si>
 </sst>
 </file>
@@ -226,13 +229,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D34" totalsRowShown="0">
-  <autoFilter ref="A1:D34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D35" totalsRowShown="0">
+  <autoFilter ref="A1:D35">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>
-  <sortState ref="A13:D34">
+  <sortState ref="A24:D35">
     <sortCondition ref="C2:C32"/>
     <sortCondition ref="A2:A32"/>
   </sortState>
@@ -509,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -691,7 +694,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -700,6 +703,9 @@
       </c>
       <c r="C13">
         <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -866,13 +872,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C26">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -903,15 +909,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C29">
         <v>15</v>
+      </c>
+      <c r="D29" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -944,10 +953,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="C32">
         <v>15</v>
@@ -969,12 +978,23 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>6</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>19</v>
       </c>
-      <c r="C34">
+      <c r="C35">
         <v>30</v>
       </c>
     </row>

</xml_diff>